<commit_message>
[github-321] Fix issue with rounding in DataFormatter. Thanks to Colin Wang. This closes #321
git-svn-id: https://svn.apache.org/repos/asf/poi/trunk@1899680 13f79535-47bb-0310-9956-ffa450edef68
</commit_message>
<xml_diff>
--- a/test-data/spreadsheet/github-321.xlsx
+++ b/test-data/spreadsheet/github-321.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2ADFE9AF-A8DC-4A0D-ABA7-CAF1420FA72D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colin/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A152773-B724-824D-A00C-E48FAD984BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" xr2:uid="{9A460EFB-F8AE-FF4D-99CE-1F5A60D3EA19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -28,9 +34,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -57,14 +66,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -372,46 +382,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7487740C-7451-9943-A628-9BEEC0E38BD2}">
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>2.04</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2.0499999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>2.0499999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2.06</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6">
-        <v>2.1</v>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>2.06</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>